<commit_message>
new R plots to look into potential learning effects, as well as overall task metrics as a function on topology. Also updated data with more codes from the insight task.
</commit_message>
<xml_diff>
--- a/results/study/MaxQDA/Coded Segments.xlsx
+++ b/results/study/MaxQDA/Coded Segments.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="206">
   <si>
     <t>Document name</t>
   </si>
@@ -376,6 +376,261 @@
   </si>
   <si>
     <t>Not a lot of interactions between SA and AS and generally not many nodes from that areas.</t>
+  </si>
+  <si>
+    <t>topology-insight\incorrect-topology-insight</t>
+  </si>
+  <si>
+    <t>Jeffrey has the most interactions with people and is not a person</t>
+  </si>
+  <si>
+    <t>there is very little institutions and a lot of people and a lot of them come from EU</t>
+  </si>
+  <si>
+    <t>There are also people with very little interactions like Nam Carlos Dominik and some others.</t>
+  </si>
+  <si>
+    <t>Jack is from South America and he is the only one from that continent plus he has an large number of followers tweets and account age.</t>
+  </si>
+  <si>
+    <t>Teo is the second account with the most followers (1181) but it doesn't have a lot of interactions (only 4) compared to users with fewer followers.</t>
+  </si>
+  <si>
+    <t>The cluster has more people than institutions and are mostly made up of NA and EU users. It has a very high average account age and follower counts but tweets are more variable.</t>
+  </si>
+  <si>
+    <t>topology-insight\neighbor-insight</t>
+  </si>
+  <si>
+    <t>topology-insight\cluster-insight</t>
+  </si>
+  <si>
+    <t>There are is a section of people who have only interacted with Jeffrey but most of the people he interacted with are from outside of the cluste</t>
+  </si>
+  <si>
+    <t>Jeffrey also has the highest follower count.</t>
+  </si>
+  <si>
+    <t>Robert also has a high number of accounts that he interacted with but they are split between the cluster and outside of it</t>
+  </si>
+  <si>
+    <t>.Krist has the most tweets</t>
+  </si>
+  <si>
+    <t>Lynn has the oldest account.</t>
+  </si>
+  <si>
+    <t>But both of these users have very few interactions within the network despite having high numbers in all fields (followers tweets account age).</t>
+  </si>
+  <si>
+    <t>When sorted by continent EU users form almost the outline of a cube through their interactions.</t>
+  </si>
+  <si>
+    <t>there's a cluster and seems to be little correlation between likesa nd followers nd mentions</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>MViews is new and has few tweets but has the 4th most followers.</t>
+  </si>
+  <si>
+    <t>North American accounts have more followers in average than European accounts</t>
+  </si>
+  <si>
+    <t>Jack is the only person from South America</t>
+  </si>
+  <si>
+    <t>Jeffrey has the most followers but less than 1000 tweets</t>
+  </si>
+  <si>
+    <t>Jeffrey has 27 neighbors meaning he interacts with his followers quite a bi</t>
+  </si>
+  <si>
+    <t>Despite only having "Robert" as a neighbor the institution Mviews has a following of over a thousand people while having almost no account activity and being very recent in the network.</t>
+  </si>
+  <si>
+    <t>everything ok</t>
+  </si>
+  <si>
+    <t>EU nodes tend to have less followers than NA nodes.</t>
+  </si>
+  <si>
+    <t>Institutions tend to have had their accounts for a shorter period</t>
+  </si>
+  <si>
+    <t>Institutes do not tend to tweet often but it could be a consequence of not having had as much time</t>
+  </si>
+  <si>
+    <t>NA also tweet a lot more than EU despite accounts being open for similar times</t>
+  </si>
+  <si>
+    <t>Jeffrey belongs to a large cluster where most interactions are directly through him</t>
+  </si>
+  <si>
+    <t>There are not many small clusters.</t>
+  </si>
+  <si>
+    <t>The nodes seem to be split between being individuals or in large clusters</t>
+  </si>
+  <si>
+    <t>Robert has interacted with almost a quarter of the total accounts on the network most of these interactions are  with people.</t>
+  </si>
+  <si>
+    <t>jeffrey and robert's interactions pattern is similar and traces a grid patterm when the order of the matrix is alphabetical.</t>
+  </si>
+  <si>
+    <t>Only one person from South America</t>
+  </si>
+  <si>
+    <t>MViews" has a very low account age but a large number of follower</t>
+  </si>
+  <si>
+    <t>Jeffrey has interacted with a lot of people despite a low tweet number</t>
+  </si>
+  <si>
+    <t>I found it interesting that most of the institutions are from the EU/NA whereas actual people were spread more globally</t>
+  </si>
+  <si>
+    <t>I was also surprised that many of the accounts with lots of followers didn't actually have that many tweets!</t>
+  </si>
+  <si>
+    <t>not sure</t>
+  </si>
+  <si>
+    <t>It's confusing and hard to look at.</t>
+  </si>
+  <si>
+    <t>unsure</t>
+  </si>
+  <si>
+    <t>mostly people with few institutions</t>
+  </si>
+  <si>
+    <t>I couldn't find any</t>
+  </si>
+  <si>
+    <t>There is a large cluster.</t>
+  </si>
+  <si>
+    <t>Gicenter has 10 interactions with itself</t>
+  </si>
+  <si>
+    <t>persons are  way more connected than institutions</t>
+  </si>
+  <si>
+    <t>in north america people are more connected than in other parts of the world</t>
+  </si>
+  <si>
+    <t>Jack seems to be the only one person from South america.</t>
+  </si>
+  <si>
+    <t>It has not neighbours from Asia</t>
+  </si>
+  <si>
+    <t>There are only three persons from Asia and in total they have very few conections.  In average they are connected only with Europe and North America.</t>
+  </si>
+  <si>
+    <t>Europeans seem to be the group with larger Account Ages.</t>
+  </si>
+  <si>
+    <t>Robert and Jeffrey seem to have the largest numbers of neighbours among the network</t>
+  </si>
+  <si>
+    <t>There is only one asian person</t>
+  </si>
+  <si>
+    <t>This person has only one immediate neighbor but is connected to Robery with the most connections in the network and so by association has many (secondary connections)</t>
+  </si>
+  <si>
+    <t>No I don't find anything particularly any different from where I started off originally. It looks about the same as I saw from the beginning of the survey.</t>
+  </si>
+  <si>
+    <t>Way too much information to peruse to find anything meaningful.</t>
+  </si>
+  <si>
+    <t>There are clusters based around certain accounts (e.g. Robert Rob and Lane). These accounts are almost always run by a person and not a business which is not something I expected.</t>
+  </si>
+  <si>
+    <t>The clusters also feature people from across the world which is another interesting feature</t>
+  </si>
+  <si>
+    <t>It becomes clear that there are several ways to identify links between individuals when they themselves may not even be aware of one another. This is probably how the US government associates people with terrorism or how facebook suggests friends that you haven't interacted with in years. It also appears that this is a test of a platform that will be provided to help them do this.</t>
+  </si>
+  <si>
+    <t>MViews has so many followers compared to the tweets and the account age but if it is an institution it might make more sense than if the account was a person.</t>
+  </si>
+  <si>
+    <t>Also usually if the account is the center of a very complicated cluster it is a person with a lot of followers.</t>
+  </si>
+  <si>
+    <t>I found that all of the institution accounts are either from North America or Europe.</t>
+  </si>
+  <si>
+    <t>Robert Rob Alex and Jeffrey seem to be pretty central figures. However it's interesting that Alex Jeffrey and Rob all have relatively few tweets</t>
+  </si>
+  <si>
+    <t>Compare that to someone like Teo who has few connections but has tons of tweets and followers</t>
+  </si>
+  <si>
+    <t>I don't really know what I'm looking for so no I don't see anything surprising or particularly interesting in the network.</t>
+  </si>
+  <si>
+    <t>MViews has a lot of followers but few tweets and his account is new</t>
+  </si>
+  <si>
+    <t>It's surprising that there are users (Marc Alex) who have few tweets and many followers.</t>
+  </si>
+  <si>
+    <t>Some people like Viau seem to have many followers but little interactions</t>
+  </si>
+  <si>
+    <t>It's interesting to see Robert a very popular and invested account have a very small account like Klaus as one of their neighbors.</t>
+  </si>
+  <si>
+    <t>Alper has a very old account and a decent number of followers/tweets but only interacts with a single person.</t>
+  </si>
+  <si>
+    <t>Lace has only interacted with one person has very few tweets and a young account but has a large number of followers</t>
+  </si>
+  <si>
+    <t>Carlose has a very old account with many tweets and a large number of followers but has only interacted with a single person</t>
+  </si>
+  <si>
+    <t>Mviews has a huge follower count on a new account with almost no tweets and only one interaction.</t>
+  </si>
+  <si>
+    <t>There don't seem to be many clusters.</t>
+  </si>
+  <si>
+    <t>Nothing surprising found</t>
+  </si>
+  <si>
+    <t>Robert Alex and Jeffrey have the most connections of all.</t>
+  </si>
+  <si>
+    <t>Nothing surprising in the network</t>
+  </si>
+  <si>
+    <t>Robert has the most activity and the biggest network</t>
+  </si>
+  <si>
+    <t>I don't know. Is there anything special?</t>
+  </si>
+  <si>
+    <t>Jan only interacts with Robert but has lots of followers and tweets and has an old account</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>In general institutions have less neighbors in the network compared to persons</t>
+  </si>
+  <si>
+    <t>Robert Alex and Jeffrey have the most followers and also the most neighbors in the network.</t>
+  </si>
+  <si>
+    <t>Everyone has interacted with each other.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +759,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C162"/>
+  <dimension ref="A1:C315"/>
   <sheetViews>
     <sheetView showGridLines="false" workbookViewId="0"/>
   </sheetViews>
@@ -993,10 +1248,10 @@
         <v>3</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45">
@@ -1007,7 +1262,7 @@
         <v>7</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46">
@@ -1015,10 +1270,10 @@
         <v>3</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47">
@@ -1029,7 +1284,7 @@
         <v>43</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48">
@@ -1037,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49">
@@ -1048,10 +1303,10 @@
         <v>3</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50">
@@ -1059,10 +1314,10 @@
         <v>3</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51">
@@ -1070,10 +1325,10 @@
         <v>3</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="52">
@@ -1084,7 +1339,7 @@
         <v>35</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53">
@@ -1095,7 +1350,7 @@
         <v>35</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54">
@@ -1103,10 +1358,10 @@
         <v>3</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55">
@@ -1114,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>51</v>
@@ -1125,10 +1380,10 @@
         <v>3</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57">
@@ -1136,10 +1391,10 @@
         <v>3</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58">
@@ -1147,10 +1402,10 @@
         <v>3</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="59">
@@ -1158,10 +1413,10 @@
         <v>3</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="60">
@@ -1169,10 +1424,10 @@
         <v>3</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61">
@@ -1180,10 +1435,10 @@
         <v>3</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62">
@@ -1191,10 +1446,10 @@
         <v>3</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63">
@@ -1205,7 +1460,7 @@
         <v>7</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64">
@@ -1213,10 +1468,10 @@
         <v>3</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="65">
@@ -1224,7 +1479,7 @@
         <v>3</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>57</v>
@@ -1235,10 +1490,10 @@
         <v>3</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67">
@@ -1246,10 +1501,10 @@
         <v>3</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68">
@@ -1257,7 +1512,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>58</v>
@@ -1268,10 +1523,10 @@
         <v>3</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70">
@@ -1279,10 +1534,10 @@
         <v>3</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71">
@@ -1290,7 +1545,7 @@
         <v>3</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>59</v>
@@ -1301,10 +1556,10 @@
         <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73">
@@ -1312,10 +1567,10 @@
         <v>3</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74">
@@ -1323,10 +1578,10 @@
         <v>3</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75">
@@ -1334,10 +1589,10 @@
         <v>3</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76">
@@ -1345,10 +1600,10 @@
         <v>3</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77">
@@ -1356,10 +1611,10 @@
         <v>3</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="78">
@@ -1367,10 +1622,10 @@
         <v>3</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79">
@@ -1381,7 +1636,7 @@
         <v>35</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80">
@@ -1389,10 +1644,10 @@
         <v>3</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81">
@@ -1403,7 +1658,7 @@
         <v>35</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82">
@@ -1411,10 +1666,10 @@
         <v>3</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83">
@@ -1422,10 +1677,10 @@
         <v>3</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="84">
@@ -1433,10 +1688,10 @@
         <v>3</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="85">
@@ -1447,7 +1702,7 @@
         <v>22</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="86">
@@ -1455,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>67</v>
@@ -1466,10 +1721,10 @@
         <v>3</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="88">
@@ -1477,10 +1732,10 @@
         <v>3</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89">
@@ -1488,10 +1743,10 @@
         <v>3</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="90">
@@ -1502,7 +1757,7 @@
         <v>7</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="91">
@@ -1510,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>70</v>
@@ -1521,7 +1776,7 @@
         <v>3</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>70</v>
@@ -1532,10 +1787,10 @@
         <v>3</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="94">
@@ -1546,7 +1801,7 @@
         <v>35</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95">
@@ -1554,10 +1809,10 @@
         <v>3</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="96">
@@ -1565,10 +1820,10 @@
         <v>3</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="97">
@@ -1576,10 +1831,10 @@
         <v>3</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="98">
@@ -1587,10 +1842,10 @@
         <v>3</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="99">
@@ -1598,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100">
@@ -1609,10 +1864,10 @@
         <v>3</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101">
@@ -1620,10 +1875,10 @@
         <v>3</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="102">
@@ -1631,10 +1886,10 @@
         <v>3</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="103">
@@ -1642,10 +1897,10 @@
         <v>3</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104">
@@ -1653,10 +1908,10 @@
         <v>3</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="105">
@@ -1667,7 +1922,7 @@
         <v>11</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="106">
@@ -1675,10 +1930,10 @@
         <v>3</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107">
@@ -1689,7 +1944,7 @@
         <v>11</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="108">
@@ -1697,10 +1952,10 @@
         <v>3</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="109">
@@ -1711,7 +1966,7 @@
         <v>11</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110">
@@ -1719,10 +1974,10 @@
         <v>3</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111">
@@ -1730,10 +1985,10 @@
         <v>3</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="112">
@@ -1741,10 +1996,10 @@
         <v>3</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="113">
@@ -1752,10 +2007,10 @@
         <v>3</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114">
@@ -1763,10 +2018,10 @@
         <v>3</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115">
@@ -1774,10 +2029,10 @@
         <v>3</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="116">
@@ -1785,10 +2040,10 @@
         <v>3</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="117">
@@ -1796,10 +2051,10 @@
         <v>3</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118">
@@ -1807,10 +2062,10 @@
         <v>3</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="119">
@@ -1818,10 +2073,10 @@
         <v>3</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="120">
@@ -1829,10 +2084,10 @@
         <v>3</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="121">
@@ -1840,10 +2095,10 @@
         <v>3</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="122">
@@ -1851,10 +2106,10 @@
         <v>3</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="123">
@@ -1862,10 +2117,10 @@
         <v>3</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="124">
@@ -1873,10 +2128,10 @@
         <v>3</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="125">
@@ -1884,10 +2139,10 @@
         <v>3</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="126">
@@ -1895,10 +2150,10 @@
         <v>3</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="127">
@@ -1906,10 +2161,10 @@
         <v>3</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="128">
@@ -1917,10 +2172,10 @@
         <v>3</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="129">
@@ -1928,10 +2183,10 @@
         <v>3</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="130">
@@ -1939,10 +2194,10 @@
         <v>3</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="131">
@@ -1950,10 +2205,10 @@
         <v>3</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="132">
@@ -1961,10 +2216,10 @@
         <v>3</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="133">
@@ -1972,10 +2227,10 @@
         <v>3</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="134">
@@ -1983,10 +2238,10 @@
         <v>3</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="135">
@@ -1994,10 +2249,10 @@
         <v>3</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="136">
@@ -2005,10 +2260,10 @@
         <v>3</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="137">
@@ -2016,10 +2271,10 @@
         <v>3</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="138">
@@ -2027,10 +2282,10 @@
         <v>3</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="139">
@@ -2038,10 +2293,10 @@
         <v>3</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="140">
@@ -2049,10 +2304,10 @@
         <v>3</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="141">
@@ -2060,10 +2315,10 @@
         <v>3</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142">
@@ -2071,10 +2326,10 @@
         <v>3</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="143">
@@ -2085,7 +2340,7 @@
         <v>7</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="144">
@@ -2093,10 +2348,10 @@
         <v>3</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="145">
@@ -2107,7 +2362,7 @@
         <v>7</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="146">
@@ -2115,10 +2370,10 @@
         <v>3</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="147">
@@ -2129,7 +2384,7 @@
         <v>7</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="148">
@@ -2137,10 +2392,10 @@
         <v>3</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="149">
@@ -2148,10 +2403,10 @@
         <v>3</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="150">
@@ -2159,7 +2414,7 @@
         <v>3</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C150" s="3" t="s">
         <v>113</v>
@@ -2170,10 +2425,10 @@
         <v>3</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="152">
@@ -2184,7 +2439,7 @@
         <v>37</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="153">
@@ -2192,10 +2447,10 @@
         <v>3</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="154">
@@ -2203,10 +2458,10 @@
         <v>3</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="155">
@@ -2217,7 +2472,7 @@
         <v>37</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="156">
@@ -2225,10 +2480,10 @@
         <v>3</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="157">
@@ -2239,7 +2494,7 @@
         <v>37</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="158">
@@ -2247,10 +2502,10 @@
         <v>3</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="159">
@@ -2258,10 +2513,10 @@
         <v>3</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="160">
@@ -2269,10 +2524,10 @@
         <v>3</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="161">
@@ -2280,10 +2535,10 @@
         <v>3</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
     </row>
     <row r="162">
@@ -2294,7 +2549,1690 @@
         <v>35</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>120</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C208" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C228" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C248" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C270" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C279" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C280" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C284" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C290" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C301" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C303" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C304" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C307" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C308" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C310" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C311" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C312" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C313" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C314" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C315" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>